<commit_message>
working on Adopted 35Ar
</commit_message>
<xml_diff>
--- a/finished/Ar35/temp/35K EC, 36Ca ECP.xlsx
+++ b/finished/Ar35/temp/35K EC, 36Ca ECP.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\Files\A35\finished\Ar35\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920F6ABC-4FEA-4415-BA95-60A1F3F2A46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C9180F-0A76-45F0-BF94-2AE2248707B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
+    <workbookView xWindow="9912" yWindow="0" windowWidth="11436" windowHeight="12000" activeTab="2" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
   </bookViews>
   <sheets>
     <sheet name="36 ECP" sheetId="1" r:id="rId1"/>
     <sheet name="35K EC" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
   <si>
     <t>Ip</t>
   </si>
@@ -110,6 +111,15 @@
   </si>
   <si>
     <t>7518(11)</t>
+  </si>
+  <si>
+    <t>35AR</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -118,7 +128,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -285,10 +295,10 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1942,7 +1952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82375D98-27FE-4F56-B80A-6CBF87E329ED}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14:H15"/>
     </sheetView>
   </sheetViews>
@@ -2401,4 +2411,103 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC3D5EA-A9A5-43EF-B54C-3B8BAAEA86C0}">
+  <dimension ref="B1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1">
+        <v>1162</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>15</v>
+      </c>
+      <c r="G1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>1756.3</v>
+      </c>
+      <c r="E2">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>17</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>1162</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>1756</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>27</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Ar35_adopted.ens with reference and multipolarity improvements
- Updated reference from 2012WA38 to 2021WA16 for Q-values
- Changed J assignment for 2982.79 keV level from "3/2+,5/2+" to "5/2+"
- Modified J assignment for 5113 keV level to "(3/2,5/2)+"
- Added missing multipolarity assignments (E2, M1) to multiple gamma transitions
- Corrected level ordering at ~6.3 MeV (6332, 6345 keV levels)
- Added XREF=A markers to proton-unbound levels at 7255, 7427 and 7509 keV
- Updated log ft value for 7509 keV level from "4.79 {i18}" to "<5.0"
- Added uncertainty indicator to XREF=A(8393?) for 8395 keV level
- Improved formatting and column alignment throughout the file
</commit_message>
<xml_diff>
--- a/finished/Ar35/temp/35K EC, 36Ca ECP.xlsx
+++ b/finished/Ar35/temp/35K EC, 36Ca ECP.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\Files\A35\finished\Ar35\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C9180F-0A76-45F0-BF94-2AE2248707B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A198A7-CB32-43C4-A39E-798E8CDD044F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9912" yWindow="0" windowWidth="11436" windowHeight="12000" activeTab="2" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
+    <workbookView xWindow="9912" yWindow="0" windowWidth="11436" windowHeight="12000" activeTab="1" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
   </bookViews>
   <sheets>
     <sheet name="36 ECP" sheetId="1" r:id="rId1"/>
     <sheet name="35K EC" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
   <si>
     <t>Ip</t>
   </si>
@@ -111,15 +110,6 @@
   </si>
   <si>
     <t>7518(11)</t>
-  </si>
-  <si>
-    <t>35AR</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1952,7 +1942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82375D98-27FE-4F56-B80A-6CBF87E329ED}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14:H15"/>
     </sheetView>
   </sheetViews>
@@ -2411,103 +2401,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC3D5EA-A9A5-43EF-B54C-3B8BAAEA86C0}">
-  <dimension ref="B1:H5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1">
-        <v>1162</v>
-      </c>
-      <c r="E1">
-        <v>8</v>
-      </c>
-      <c r="F1">
-        <v>15</v>
-      </c>
-      <c r="G1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2">
-        <v>1756.3</v>
-      </c>
-      <c r="E2">
-        <v>14</v>
-      </c>
-      <c r="F2">
-        <v>17</v>
-      </c>
-      <c r="G2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4">
-        <v>1162</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>11</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5">
-        <v>1756</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>27</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added 35Ca 3 datasets
</commit_message>
<xml_diff>
--- a/finished/Ar35/temp/35K EC, 36Ca ECP.xlsx
+++ b/finished/Ar35/temp/35K EC, 36Ca ECP.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\X\ND\Files\A35\finished\Ar35\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8119FEC6-683B-4B74-8228-A8B6E243B59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6BF170-3188-4BC6-98F5-D72A1A782324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{80E8E01B-A04B-4992-8B74-8F4DE158A446}"/>
   </bookViews>
   <sheets>
     <sheet name="36 ECP" sheetId="1" r:id="rId1"/>
     <sheet name="35K EC" sheetId="2" r:id="rId2"/>
+    <sheet name="35Ca EC" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="79">
   <si>
     <t>Ip</t>
   </si>
@@ -116,6 +117,162 @@
   </si>
   <si>
     <t>Batch</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>Eₚ (keV)</t>
+  </si>
+  <si>
+    <t>xᵢ (%)</t>
+  </si>
+  <si>
+    <t>Decay mode</t>
+  </si>
+  <si>
+    <t>1427(5)</t>
+  </si>
+  <si>
+    <t>48.5(1.3)</t>
+  </si>
+  <si>
+    <t>p₀</t>
+  </si>
+  <si>
+    <t>8.4(6)</t>
+  </si>
+  <si>
+    <t>p₁, p₂, p₃</t>
+  </si>
+  <si>
+    <t>2727(13)</t>
+  </si>
+  <si>
+    <t>6.0(5)</t>
+  </si>
+  <si>
+    <t>p₁</t>
+  </si>
+  <si>
+    <t>2.2(3)</t>
+  </si>
+  <si>
+    <t>3592(25)</t>
+  </si>
+  <si>
+    <t>3.0(3)</t>
+  </si>
+  <si>
+    <t>3822(36)</t>
+  </si>
+  <si>
+    <t>3.8(3)</t>
+  </si>
+  <si>
+    <t>4041(71)</t>
+  </si>
+  <si>
+    <t>2.9(3)</t>
+  </si>
+  <si>
+    <t>4305(26)ᵇ</t>
+  </si>
+  <si>
+    <t>4.2(3)</t>
+  </si>
+  <si>
+    <t>2p₀</t>
+  </si>
+  <si>
+    <t>4570(48)</t>
+  </si>
+  <si>
+    <t>4754(38)</t>
+  </si>
+  <si>
+    <t>4.2(4)</t>
+  </si>
+  <si>
+    <t>5018(71)</t>
+  </si>
+  <si>
+    <t>3.9(3)</t>
+  </si>
+  <si>
+    <t>5294(48)</t>
+  </si>
+  <si>
+    <t>0.72(18)</t>
+  </si>
+  <si>
+    <t>5466(48)</t>
+  </si>
+  <si>
+    <t>0.61(15)</t>
+  </si>
+  <si>
+    <t>5616(37)</t>
+  </si>
+  <si>
+    <t>1.43(17)</t>
+  </si>
+  <si>
+    <t>5834(60)</t>
+  </si>
+  <si>
+    <t>1.40(19)</t>
+  </si>
+  <si>
+    <t>1.09(17)</t>
+  </si>
+  <si>
+    <t>6783(22)</t>
+  </si>
+  <si>
+    <t>3.8(2)</t>
+  </si>
+  <si>
+    <t>1.1(2)</t>
+  </si>
+  <si>
+    <t>8802(89)</t>
+  </si>
+  <si>
+    <t>0.41(6)</t>
+  </si>
+  <si>
+    <t>1909–2647</t>
+  </si>
+  <si>
+    <t>2947–3500</t>
+  </si>
+  <si>
+    <t>5983–6649</t>
+  </si>
+  <si>
+    <t>7131–7887</t>
+  </si>
+  <si>
+    <t>Ecm</t>
+  </si>
+  <si>
+    <t>Sp(35K)</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>gs</t>
+  </si>
+  <si>
+    <t>σEp</t>
   </si>
 </sst>
 </file>
@@ -126,7 +283,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +367,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -304,6 +467,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -635,7 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73FCEC0C-CCF2-405C-89E2-FB3C4ADFF355}">
   <dimension ref="A1:AG47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
@@ -2586,4 +2758,856 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0A5003-67F5-4A2F-AC32-71311414C574}">
+  <dimension ref="A1:M28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="8.88671875" style="25"/>
+    <col min="13" max="13" width="3.44140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E1" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="25">
+        <v>83.6</v>
+      </c>
+      <c r="G1" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="J1" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="K1" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="L1" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I2" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="25">
+        <v>2091.1</v>
+      </c>
+      <c r="K3" s="27">
+        <v>3287.7</v>
+      </c>
+      <c r="L3" s="25">
+        <v>3873</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <v>1</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="25" t="str">
+        <f>LEFT(B4,4)</f>
+        <v>1427</v>
+      </c>
+      <c r="F4" s="25">
+        <f>E4/34*35</f>
+        <v>1468.9705882352941</v>
+      </c>
+      <c r="G4" s="25" t="str">
+        <f>MID(B4,6,1)</f>
+        <v>5</v>
+      </c>
+      <c r="H4" s="26">
+        <f>G4/34*35</f>
+        <v>5.1470588235294121</v>
+      </c>
+      <c r="I4" s="26">
+        <f>$F4+$F$1</f>
+        <v>1552.5705882352941</v>
+      </c>
+      <c r="M4" s="26">
+        <f>SQRT($H4^2+G$1^2)</f>
+        <v>5.1712875121068231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="25" t="str">
+        <f>LEFT(B5,4)</f>
+        <v>2727</v>
+      </c>
+      <c r="F5" s="25">
+        <f t="shared" ref="F5:F15" si="0">E5/34*35</f>
+        <v>2807.205882352941</v>
+      </c>
+      <c r="G5" s="25" t="str">
+        <f>MID(B5,6,2)</f>
+        <v>13</v>
+      </c>
+      <c r="H5" s="26">
+        <f t="shared" ref="H5:H17" si="1">G5/34*35</f>
+        <v>13.382352941176469</v>
+      </c>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26">
+        <f>$F5+$F$1+J$3</f>
+        <v>4981.9058823529413</v>
+      </c>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26">
+        <f t="shared" ref="M5:M17" si="2">SQRT($H5^2+G$1^2)</f>
+        <v>13.39169034297816</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <v>5</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="25" t="str">
+        <f>LEFT(B6,4)</f>
+        <v>3592</v>
+      </c>
+      <c r="F6" s="25">
+        <f t="shared" si="0"/>
+        <v>3697.6470588235293</v>
+      </c>
+      <c r="G6" s="25" t="str">
+        <f t="shared" ref="G6:G17" si="3">MID(B6,6,2)</f>
+        <v>25</v>
+      </c>
+      <c r="H6" s="26">
+        <f t="shared" si="1"/>
+        <v>25.735294117647062</v>
+      </c>
+      <c r="I6" s="26">
+        <f>$F6+$F$1</f>
+        <v>3781.2470588235292</v>
+      </c>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26">
+        <f t="shared" si="2"/>
+        <v>25.740150802235007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
+        <v>6</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="25" t="str">
+        <f>LEFT(B7,4)</f>
+        <v>3822</v>
+      </c>
+      <c r="F7" s="25">
+        <f t="shared" si="0"/>
+        <v>3934.411764705882</v>
+      </c>
+      <c r="G7" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="H7" s="26">
+        <f t="shared" si="1"/>
+        <v>37.058823529411768</v>
+      </c>
+      <c r="I7" s="26">
+        <f>$F7+$F$1</f>
+        <v>4018.0117647058819</v>
+      </c>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26">
+        <f t="shared" si="2"/>
+        <v>37.062196391796363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <v>7</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="25" t="str">
+        <f>LEFT(B8,4)</f>
+        <v>4041</v>
+      </c>
+      <c r="F8" s="25">
+        <f t="shared" si="0"/>
+        <v>4159.8529411764712</v>
+      </c>
+      <c r="G8" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="H8" s="26">
+        <f t="shared" si="1"/>
+        <v>73.088235294117652</v>
+      </c>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26">
+        <f>$F8+$F$1+J$3</f>
+        <v>6334.552941176471</v>
+      </c>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26">
+        <f t="shared" si="2"/>
+        <v>73.089945535677515</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <v>9</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="25" t="str">
+        <f>LEFT(B9,4)</f>
+        <v>4570</v>
+      </c>
+      <c r="F9" s="25">
+        <f t="shared" si="0"/>
+        <v>4704.411764705882</v>
+      </c>
+      <c r="G9" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="H9" s="26">
+        <f t="shared" si="1"/>
+        <v>49.411764705882355</v>
+      </c>
+      <c r="I9" s="26">
+        <f>$F9+$F$1</f>
+        <v>4788.0117647058823</v>
+      </c>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26">
+        <f t="shared" si="2"/>
+        <v>49.414294403031612</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <v>10</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="25" t="str">
+        <f>LEFT(B10,4)</f>
+        <v>4754</v>
+      </c>
+      <c r="F10" s="25">
+        <f t="shared" si="0"/>
+        <v>4893.823529411764</v>
+      </c>
+      <c r="G10" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="H10" s="26">
+        <f t="shared" si="1"/>
+        <v>39.117647058823529</v>
+      </c>
+      <c r="I10" s="26">
+        <f>$F10+$F$1</f>
+        <v>4977.4235294117643</v>
+      </c>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26">
+        <f t="shared" si="2"/>
+        <v>39.120842417037558</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <v>11</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="25" t="str">
+        <f>LEFT(B11,4)</f>
+        <v>5018</v>
+      </c>
+      <c r="F11" s="25">
+        <f t="shared" si="0"/>
+        <v>5165.588235294118</v>
+      </c>
+      <c r="G11" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="H11" s="26">
+        <f t="shared" si="1"/>
+        <v>73.088235294117652</v>
+      </c>
+      <c r="I11" s="26">
+        <f>$F11+$F$1</f>
+        <v>5249.1882352941184</v>
+      </c>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26">
+        <f t="shared" si="2"/>
+        <v>73.089945535677515</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <v>12</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="25" t="str">
+        <f>LEFT(B12,4)</f>
+        <v>5294</v>
+      </c>
+      <c r="F12" s="25">
+        <f t="shared" si="0"/>
+        <v>5449.7058823529414</v>
+      </c>
+      <c r="G12" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="H12" s="26">
+        <f t="shared" si="1"/>
+        <v>49.411764705882355</v>
+      </c>
+      <c r="I12" s="26">
+        <f>$F12+$F$1</f>
+        <v>5533.3058823529418</v>
+      </c>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26">
+        <f t="shared" si="2"/>
+        <v>49.414294403031612</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <v>13</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="25" t="str">
+        <f>LEFT(B13,4)</f>
+        <v>5466</v>
+      </c>
+      <c r="F13" s="25">
+        <f t="shared" si="0"/>
+        <v>5626.7647058823522</v>
+      </c>
+      <c r="G13" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="H13" s="26">
+        <f t="shared" si="1"/>
+        <v>49.411764705882355</v>
+      </c>
+      <c r="I13" s="26">
+        <f>$F13+$F$1</f>
+        <v>5710.3647058823526</v>
+      </c>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26">
+        <f t="shared" si="2"/>
+        <v>49.414294403031612</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <v>14</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="25" t="str">
+        <f>LEFT(B14,4)</f>
+        <v>5616</v>
+      </c>
+      <c r="F14" s="25">
+        <f t="shared" si="0"/>
+        <v>5781.176470588236</v>
+      </c>
+      <c r="G14" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="H14" s="26">
+        <f t="shared" si="1"/>
+        <v>38.088235294117645</v>
+      </c>
+      <c r="I14" s="26">
+        <f>$F14+$F$1</f>
+        <v>5864.7764705882364</v>
+      </c>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26">
+        <f t="shared" si="2"/>
+        <v>38.09151700602208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <v>15</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="25" t="str">
+        <f>LEFT(B15,4)</f>
+        <v>5834</v>
+      </c>
+      <c r="F15" s="25">
+        <f t="shared" si="0"/>
+        <v>6005.588235294118</v>
+      </c>
+      <c r="G15" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="H15" s="26">
+        <f t="shared" si="1"/>
+        <v>61.764705882352942</v>
+      </c>
+      <c r="I15" s="26">
+        <f>$F15+$F$1</f>
+        <v>6089.1882352941184</v>
+      </c>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26">
+        <f t="shared" si="2"/>
+        <v>61.766729658721317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <v>17</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="25" t="str">
+        <f t="shared" ref="E16" si="4">LEFT(B16,4)</f>
+        <v>6783</v>
+      </c>
+      <c r="F16" s="25">
+        <f>E16/34*35</f>
+        <v>6982.5</v>
+      </c>
+      <c r="G16" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="H16" s="26">
+        <f t="shared" si="1"/>
+        <v>22.647058823529413</v>
+      </c>
+      <c r="I16" s="26"/>
+      <c r="J16" s="25">
+        <f>$E16+$F$1+J$3</f>
+        <v>8957.7000000000007</v>
+      </c>
+      <c r="M16" s="26">
+        <f t="shared" si="2"/>
+        <v>22.652577631616261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <v>19</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="25" t="str">
+        <f>LEFT(B17,4)</f>
+        <v>8802</v>
+      </c>
+      <c r="F17" s="25">
+        <f>E17/34*35</f>
+        <v>9060.8823529411766</v>
+      </c>
+      <c r="G17" s="25" t="str">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+      <c r="H17" s="26">
+        <f t="shared" si="1"/>
+        <v>91.617647058823536</v>
+      </c>
+      <c r="I17" s="26">
+        <f>$E17/34*35+$F$1</f>
+        <v>9144.4823529411769</v>
+      </c>
+      <c r="M17" s="26">
+        <f>SQRT($H17^2+G$1^2)</f>
+        <v>91.61901141463575</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <v>8</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="25" t="str">
+        <f>LEFT(B24,4)</f>
+        <v>4305</v>
+      </c>
+      <c r="F24" s="25">
+        <f>E24/34*35</f>
+        <v>4431.6176470588234</v>
+      </c>
+      <c r="G24" s="26">
+        <f>$E24/34*35+$F$1</f>
+        <v>4515.2176470588238</v>
+      </c>
+      <c r="H24" s="25">
+        <f>$E24+$F$1+J$3</f>
+        <v>6479.7000000000007</v>
+      </c>
+      <c r="I24" s="25">
+        <f>$E24+$F$1+K$3</f>
+        <v>7676.3</v>
+      </c>
+      <c r="J24" s="25">
+        <f>$E24+$F$1+L$3</f>
+        <v>8261.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
+        <v>2</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="25" t="str">
+        <f>LEFT(B25,4)</f>
+        <v>1909</v>
+      </c>
+      <c r="F25" s="25">
+        <f>E25/34*35</f>
+        <v>1965.1470588235295</v>
+      </c>
+      <c r="G25" s="26">
+        <f>$E25/34*35+$F$1</f>
+        <v>2048.7470588235296</v>
+      </c>
+      <c r="H25" s="25">
+        <f>$E25+$F$1+J$3</f>
+        <v>4083.7</v>
+      </c>
+      <c r="I25" s="25">
+        <f>$E25+$F$1+K$3</f>
+        <v>5280.2999999999993</v>
+      </c>
+      <c r="J25" s="25">
+        <f>$E25+$F$1+L$3</f>
+        <v>5865.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <v>4</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="25" t="str">
+        <f>LEFT(B26,4)</f>
+        <v>2947</v>
+      </c>
+      <c r="F26" s="25">
+        <f>E26/34*35</f>
+        <v>3033.6764705882351</v>
+      </c>
+      <c r="G26" s="26">
+        <f>$E26/34*35+$F$1</f>
+        <v>3117.276470588235</v>
+      </c>
+      <c r="H26" s="25">
+        <f>$E26+$F$1+J$3</f>
+        <v>5121.7</v>
+      </c>
+      <c r="I26" s="25">
+        <f>$E26+$F$1+K$3</f>
+        <v>6318.2999999999993</v>
+      </c>
+      <c r="J26" s="25">
+        <f>$E26+$F$1+L$3</f>
+        <v>6903.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <v>16</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="25" t="str">
+        <f>LEFT(B27,4)</f>
+        <v>5983</v>
+      </c>
+      <c r="F27" s="25">
+        <f>E27/34*35</f>
+        <v>6158.9705882352937</v>
+      </c>
+      <c r="G27" s="26">
+        <f>$E27/34*35+$F$1</f>
+        <v>6242.5705882352941</v>
+      </c>
+      <c r="H27" s="25">
+        <f>$E27+$F$1+J$3</f>
+        <v>8157.7000000000007</v>
+      </c>
+      <c r="I27" s="25">
+        <f>$E27+$F$1+K$3</f>
+        <v>9354.2999999999993</v>
+      </c>
+      <c r="J27" s="25">
+        <f>$E27+$F$1+L$3</f>
+        <v>9939.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <v>18</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="25" t="str">
+        <f>LEFT(B28,4)</f>
+        <v>7131</v>
+      </c>
+      <c r="F28" s="25">
+        <f>E28/34*35</f>
+        <v>7340.7352941176478</v>
+      </c>
+      <c r="G28" s="26">
+        <f>$E28/34*35+$F$1</f>
+        <v>7424.3352941176481</v>
+      </c>
+      <c r="H28" s="25">
+        <f>$E28+$F$1+J$3</f>
+        <v>9305.7000000000007</v>
+      </c>
+      <c r="I28" s="25">
+        <f>$E28+$F$1+K$3</f>
+        <v>10502.3</v>
+      </c>
+      <c r="J28" s="25">
+        <f>$E28+$F$1+L$3</f>
+        <v>11087.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>